<commit_message>
lets aplicate with normalization in database into 3NF
</commit_message>
<xml_diff>
--- a/Tablas_db.xlsx
+++ b/Tablas_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\DEVELOPER\sql_all\db_empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66655E7A-F455-422F-A603-3A83003CE3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197E0815-672B-421C-9EE5-B1BA23C0BFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{A9BB755E-2C6C-44DD-A85D-FEE8E02A20BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{A9BB755E-2C6C-44DD-A85D-FEE8E02A20BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,26 +19,20 @@
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
     <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
     <sheet name="Hoja6" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja7-2fn" sheetId="7" r:id="rId7"/>
+    <sheet name="Hoja8-3fn" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="80">
   <si>
     <t>USERS</t>
   </si>
@@ -272,6 +266,12 @@
   </si>
   <si>
     <t>taggable_type</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>categoria_id</t>
   </si>
 </sst>
 </file>
@@ -380,13 +380,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,15 +407,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -739,24 +740,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -803,28 +804,28 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -875,24 +876,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -939,28 +940,28 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1052,7 +1053,7 @@
   <dimension ref="C4:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,34 +1066,34 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="H4" s="8" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="H5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1157,16 +1158,16 @@
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1237,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F7781B-EB39-4F22-9599-2D455F9EF6CF}">
   <dimension ref="C3:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,60 +1255,60 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="8" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="H3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="L3" s="4" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="L3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="L4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1456,7 +1457,7 @@
   <dimension ref="B3:Q8"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L7"/>
+      <selection activeCell="H3" sqref="H3:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,68 +1471,68 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="4" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="H3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
-      <c r="N3" s="8" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8"/>
+      <c r="N3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" s="7" t="s">
+      <c r="N4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1575,7 +1576,7 @@
       <c r="P5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="Q5" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1619,7 +1620,7 @@
       <c r="P6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1663,7 +1664,7 @@
       <c r="P7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1714,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6FC565-E3F7-42D6-A0EE-17D18A67E21F}">
   <dimension ref="B3:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,46 +1728,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="8" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="H3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1795,7 +1796,7 @@
       <c r="J5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1824,7 +1825,7 @@
       <c r="J6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1853,7 +1854,7 @@
       <c r="J7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1875,34 +1876,34 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
@@ -1920,7 +1921,7 @@
       <c r="G14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
@@ -1938,7 +1939,7 @@
       <c r="G15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
@@ -1956,7 +1957,7 @@
       <c r="G16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
@@ -1975,4 +1976,328 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB44113-3694-48FB-9D1D-86E428E34F8D}">
+  <dimension ref="B4:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="G4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="G4:K4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{46611D0C-392B-42A8-8FF3-E7A3DF7DCF29}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{504A5D26-E804-40CF-9D26-919DE827B047}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{9671AC6B-ACA2-4BAF-AA5D-5120979057F3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C6EF55-987A-4192-B576-4916B94FBED0}">
+  <dimension ref="C3:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="I3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>